<commit_message>
Some cleanup of the code.
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MatlabCode\projects\TMEModeling\TMEModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313378CB-899F-408D-9FA1-3EDA2198778B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984D3559-DA1F-46D9-A9DA-72857AFD5212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,12 +60,6 @@
     <t>fixFluxes</t>
   </si>
   <si>
-    <t>genFig2_3ABData</t>
-  </si>
-  <si>
-    <t>genFig5Data</t>
-  </si>
-  <si>
     <t>increaseMetConstraints</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>TC006, + the results look reasonable</t>
   </si>
   <si>
-    <t>This code is not explictly tested. It is much code, but quite trivial, and we have investigated the results throroughly when trying to understand what is happening in the model, so we deem it to be safe.</t>
-  </si>
-  <si>
     <t>We don't test this function, it is rather straight-forward and produces reasonable results.</t>
   </si>
   <si>
@@ -224,6 +215,15 @@
   </si>
   <si>
     <t>Implicitly tested with TC003 and in all simulations. We didn't explicitly test the blood model, but it is trivial and gives expected results.</t>
+  </si>
+  <si>
+    <t>This code is not explictly tested. It is much code, but quite trivial, and we have investigated the results throroughly when trying to understand what is happening in the model, so we deem it to be safe. The code for investigating complex II in reverse across the hypoxia range is very similar to that of GenFig1-2ABData.m.</t>
+  </si>
+  <si>
+    <t>genFig1_2ABData</t>
+  </si>
+  <si>
+    <t>genFig3Data</t>
   </si>
 </sst>
 </file>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -594,7 +594,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -615,10 +615,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,224 +642,224 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
         <v>56</v>
-      </c>
-      <c r="B38" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some changes for the revision
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MatlabCode\projects\TMEModeling\TMEModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFB6EAE-2763-4ED6-B017-36866BCEBDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2892D90-340F-4386-B9DE-08928904C9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Verification</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>Tested by two tests in runRxnDependenceTest.m. In addition, the code has been reviewed.</t>
+  </si>
+  <si>
+    <t>CompFullAndLight.m</t>
+  </si>
+  <si>
+    <t>Only a small script taken from the GECKO 3 tutorial, no tests deemed necessary.</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,63 +614,63 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -672,79 +678,79 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
@@ -752,23 +758,23 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>39</v>
@@ -776,68 +782,68 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>22</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
         <v>58</v>
@@ -845,7 +851,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B38" t="s">
         <v>58</v>
@@ -853,15 +859,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
         <v>57</v>
@@ -869,17 +875,25 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>54</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>